<commit_message>
Ca_v1_1 magyarítás eső körben készen
</commit_message>
<xml_diff>
--- a/HUniclass2015_Ca_v1_1.xlsx
+++ b/HUniclass2015_Ca_v1_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cs/Sites/MAKR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2668633-F53D-CB47-84D5-1A0AC1E1A221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B364BC-6D4A-4C48-82AB-456243AF32A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34540" windowHeight="18980" xr2:uid="{E6D54E73-570D-4BEC-A770-1DA5B9EBA596}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="277">
   <si>
     <t>Kód</t>
   </si>
@@ -115,12 +115,6 @@
     <t>Logó</t>
   </si>
   <si>
-    <t>Nézetablakok</t>
-  </si>
-  <si>
-    <t>Felhők és jelölések tartása</t>
-  </si>
-  <si>
     <t>Felülvizsgálatok</t>
   </si>
   <si>
@@ -130,9 +124,6 @@
     <t>Blokkok és cellák</t>
   </si>
   <si>
-    <t>Felhők és jelölések</t>
-  </si>
-  <si>
     <t>Állapotbélyegzők</t>
   </si>
   <si>
@@ -181,9 +172,6 @@
     <t>Terület kitöltése</t>
   </si>
   <si>
-    <t>Hatch határok</t>
-  </si>
-  <si>
     <t>Mintázat</t>
   </si>
   <si>
@@ -202,18 +190,9 @@
     <t>Kereszthivatkozások</t>
   </si>
   <si>
-    <t>Kulcsterv</t>
-  </si>
-  <si>
-    <t>Legendák</t>
-  </si>
-  <si>
     <t>Északi pont</t>
   </si>
   <si>
-    <t>Cím megjegyzés</t>
-  </si>
-  <si>
     <t>Beillesztések</t>
   </si>
   <si>
@@ -232,9 +211,6 @@
     <t>Kijelölés</t>
   </si>
   <si>
-    <t>Kiegyenlítések és felülnézettségek</t>
-  </si>
-  <si>
     <t>Vízszintes igazítás</t>
   </si>
   <si>
@@ -863,6 +839,39 @@
   </si>
   <si>
     <t>External reference information</t>
+  </si>
+  <si>
+    <t>Jelölők</t>
+  </si>
+  <si>
+    <t>Felhőjelölők</t>
+  </si>
+  <si>
+    <t>Kitöltők</t>
+  </si>
+  <si>
+    <t>Kitöltés határok</t>
+  </si>
+  <si>
+    <t>Hibajelölők</t>
+  </si>
+  <si>
+    <t>Méretarány</t>
+  </si>
+  <si>
+    <t>Jemagyarázat</t>
+  </si>
+  <si>
+    <t>Helyszínrajz</t>
+  </si>
+  <si>
+    <t>Cím</t>
+  </si>
+  <si>
+    <t>Kiegyenlítések és felülnézetek</t>
+  </si>
+  <si>
+    <t>Leírás</t>
   </si>
 </sst>
 </file>
@@ -1238,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B96C505-3159-4C65-919E-CC7A86783427}">
   <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="D107" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="J131" sqref="J131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1261,10 +1270,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -1282,13 +1291,13 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1300,7 +1309,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -1309,19 +1318,19 @@
         <v>21</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
-        <f t="shared" ref="A2:A8" si="0">CONCATENATE(B3,"-",D3,IF(ISBLANK(E3),"",CONCATENATE("-",E3)),IF(ISBLANK(F3),"",CONCATENATE("-",F3)),IF(ISBLANK(G3),"",CONCATENATE("-",G3)),IF(ISBLANK(H3),"",CONCATENATE("-",H3)))</f>
+        <f t="shared" ref="A3:A8" si="0">CONCATENATE(B3,"-",D3,IF(ISBLANK(E3),"",CONCATENATE("-",E3)),IF(ISBLANK(F3),"",CONCATENATE("-",F3)),IF(ISBLANK(G3),"",CONCATENATE("-",G3)),IF(ISBLANK(H3),"",CONCATENATE("-",H3)))</f>
         <v>Ca-10-20</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -1333,7 +1342,7 @@
         <v>22</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1345,7 +1354,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
@@ -1360,7 +1369,7 @@
         <v>23</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1372,7 +1381,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
@@ -1384,10 +1393,10 @@
         <v>19</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1399,7 +1408,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
@@ -1408,10 +1417,10 @@
         <v>14</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>25</v>
+        <v>266</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1423,7 +1432,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
@@ -1432,10 +1441,10 @@
         <v>16</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1447,7 +1456,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
@@ -1459,10 +1468,10 @@
         <v>18</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1474,7 +1483,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
@@ -1486,10 +1495,10 @@
         <v>9</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1501,7 +1510,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
@@ -1513,10 +1522,10 @@
         <v>6</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>29</v>
+        <v>267</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1528,7 +1537,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
@@ -1537,10 +1546,10 @@
         <v>11</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1552,16 +1561,16 @@
         <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1573,7 +1582,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -1582,10 +1591,10 @@
         <v>9</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1597,7 +1606,7 @@
         <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
@@ -1609,10 +1618,10 @@
         <v>14</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1624,7 +1633,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
@@ -1636,10 +1645,10 @@
         <v>13</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1651,7 +1660,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -1663,10 +1672,10 @@
         <v>15</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1678,7 +1687,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
@@ -1687,13 +1696,13 @@
         <v>9</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1705,7 +1714,7 @@
         <v>20</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>6</v>
@@ -1717,10 +1726,10 @@
         <v>16</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1732,7 +1741,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>6</v>
@@ -1744,10 +1753,10 @@
         <v>12</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1759,7 +1768,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>6</v>
@@ -1768,13 +1777,13 @@
         <v>9</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1786,7 +1795,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>6</v>
@@ -1795,10 +1804,10 @@
         <v>6</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1810,7 +1819,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>6</v>
@@ -1819,10 +1828,10 @@
         <v>8</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1834,7 +1843,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>6</v>
@@ -1846,10 +1855,10 @@
         <v>15</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1861,7 +1870,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>6</v>
@@ -1873,10 +1882,10 @@
         <v>19</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1888,7 +1897,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>6</v>
@@ -1897,10 +1906,10 @@
         <v>14</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>44</v>
+        <v>268</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -1912,7 +1921,7 @@
         <v>20</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>6</v>
@@ -1924,10 +1933,10 @@
         <v>18</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -1939,7 +1948,7 @@
         <v>20</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>6</v>
@@ -1951,10 +1960,10 @@
         <v>10</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>46</v>
+        <v>269</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1966,7 +1975,7 @@
         <v>20</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>6</v>
@@ -1978,10 +1987,10 @@
         <v>17</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1993,7 +2002,7 @@
         <v>20</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>6</v>
@@ -2005,10 +2014,10 @@
         <v>11</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -2020,7 +2029,7 @@
         <v>20</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>6</v>
@@ -2029,10 +2038,10 @@
         <v>16</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>49</v>
+        <v>270</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -2044,7 +2053,7 @@
         <v>20</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>6</v>
@@ -2056,10 +2065,10 @@
         <v>6</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -2071,7 +2080,7 @@
         <v>20</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>6</v>
@@ -2080,10 +2089,10 @@
         <v>11</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -2095,7 +2104,7 @@
         <v>20</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>6</v>
@@ -2107,10 +2116,10 @@
         <v>9</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>51</v>
+        <v>271</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -2122,7 +2131,7 @@
         <v>20</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>6</v>
@@ -2134,10 +2143,10 @@
         <v>7</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -2149,7 +2158,7 @@
         <v>20</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>6</v>
@@ -2161,10 +2170,10 @@
         <v>14</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>53</v>
+        <v>273</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -2176,7 +2185,7 @@
         <v>20</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>6</v>
@@ -2188,10 +2197,10 @@
         <v>15</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>54</v>
+        <v>272</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -2203,7 +2212,7 @@
         <v>20</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>6</v>
@@ -2212,13 +2221,13 @@
         <v>11</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -2230,19 +2239,19 @@
         <v>20</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>56</v>
+        <v>274</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -2254,16 +2263,16 @@
         <v>20</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -2275,7 +2284,7 @@
         <v>20</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>8</v>
@@ -2284,10 +2293,10 @@
         <v>6</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -2299,7 +2308,7 @@
         <v>20</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>8</v>
@@ -2308,10 +2317,10 @@
         <v>8</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -2323,7 +2332,7 @@
         <v>20</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>8</v>
@@ -2332,10 +2341,10 @@
         <v>14</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -2347,7 +2356,7 @@
         <v>20</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>8</v>
@@ -2356,10 +2365,10 @@
         <v>17</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -2371,19 +2380,19 @@
         <v>20</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -2395,16 +2404,16 @@
         <v>20</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -2416,7 +2425,7 @@
         <v>20</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>10</v>
@@ -2425,10 +2434,10 @@
         <v>9</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>63</v>
+        <v>275</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -2440,7 +2449,7 @@
         <v>20</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>10</v>
@@ -2452,10 +2461,10 @@
         <v>14</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -2467,7 +2476,7 @@
         <v>20</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>10</v>
@@ -2479,10 +2488,10 @@
         <v>11</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -2494,7 +2503,7 @@
         <v>20</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>10</v>
@@ -2503,13 +2512,13 @@
         <v>9</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -2521,7 +2530,7 @@
         <v>20</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>10</v>
@@ -2530,10 +2539,10 @@
         <v>6</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -2545,7 +2554,7 @@
         <v>20</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>10</v>
@@ -2554,10 +2563,10 @@
         <v>8</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -2569,7 +2578,7 @@
         <v>20</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>10</v>
@@ -2578,10 +2587,10 @@
         <v>14</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -2593,7 +2602,7 @@
         <v>20</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>10</v>
@@ -2605,10 +2614,10 @@
         <v>6</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -2620,7 +2629,7 @@
         <v>20</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>10</v>
@@ -2632,10 +2641,10 @@
         <v>11</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -2647,7 +2656,7 @@
         <v>20</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>10</v>
@@ -2656,10 +2665,10 @@
         <v>17</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -2671,7 +2680,7 @@
         <v>20</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>10</v>
@@ -2680,10 +2689,10 @@
         <v>11</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -2695,7 +2704,7 @@
         <v>20</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>10</v>
@@ -2704,13 +2713,13 @@
         <v>11</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -2722,7 +2731,7 @@
         <v>20</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>10</v>
@@ -2734,10 +2743,10 @@
         <v>17</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -2749,7 +2758,7 @@
         <v>20</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>10</v>
@@ -2761,10 +2770,10 @@
         <v>11</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -2776,7 +2785,7 @@
         <v>20</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>10</v>
@@ -2788,10 +2797,10 @@
         <v>12</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -2803,7 +2812,7 @@
         <v>20</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>10</v>
@@ -2812,13 +2821,13 @@
         <v>11</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -2830,16 +2839,16 @@
         <v>20</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -2851,7 +2860,7 @@
         <v>20</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>14</v>
@@ -2860,10 +2869,10 @@
         <v>7</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -2875,7 +2884,7 @@
         <v>20</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>14</v>
@@ -2887,10 +2896,10 @@
         <v>15</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
@@ -2902,7 +2911,7 @@
         <v>20</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>14</v>
@@ -2911,13 +2920,13 @@
         <v>7</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
@@ -2929,7 +2938,7 @@
         <v>20</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>14</v>
@@ -2938,10 +2947,10 @@
         <v>6</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -2953,7 +2962,7 @@
         <v>20</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>14</v>
@@ -2962,10 +2971,10 @@
         <v>15</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -2977,16 +2986,16 @@
         <v>20</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
@@ -2998,7 +3007,7 @@
         <v>20</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>15</v>
@@ -3007,10 +3016,10 @@
         <v>9</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
@@ -3022,7 +3031,7 @@
         <v>20</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>15</v>
@@ -3034,10 +3043,10 @@
         <v>9</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -3049,7 +3058,7 @@
         <v>20</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>15</v>
@@ -3061,10 +3070,10 @@
         <v>16</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
@@ -3076,7 +3085,7 @@
         <v>20</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>15</v>
@@ -3085,10 +3094,10 @@
         <v>15</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
@@ -3100,7 +3109,7 @@
         <v>20</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>15</v>
@@ -3109,10 +3118,10 @@
         <v>17</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -3124,19 +3133,19 @@
         <v>20</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -3148,7 +3157,7 @@
         <v>20</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>15</v>
@@ -3157,10 +3166,10 @@
         <v>19</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -3172,16 +3181,16 @@
         <v>20</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -3193,7 +3202,7 @@
         <v>20</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>17</v>
@@ -3202,10 +3211,10 @@
         <v>6</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -3217,7 +3226,7 @@
         <v>20</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>17</v>
@@ -3226,10 +3235,10 @@
         <v>8</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -3241,7 +3250,7 @@
         <v>20</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>17</v>
@@ -3250,10 +3259,10 @@
         <v>14</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
@@ -3265,7 +3274,7 @@
         <v>20</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>17</v>
@@ -3277,10 +3286,10 @@
         <v>7</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
@@ -3292,7 +3301,7 @@
         <v>20</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>17</v>
@@ -3304,10 +3313,10 @@
         <v>6</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -3319,7 +3328,7 @@
         <v>20</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>17</v>
@@ -3331,10 +3340,10 @@
         <v>8</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -3346,7 +3355,7 @@
         <v>20</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>17</v>
@@ -3355,10 +3364,10 @@
         <v>13</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -3370,7 +3379,7 @@
         <v>20</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>17</v>
@@ -3382,10 +3391,10 @@
         <v>6</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
@@ -3397,7 +3406,7 @@
         <v>20</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>17</v>
@@ -3409,10 +3418,10 @@
         <v>17</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -3424,7 +3433,7 @@
         <v>20</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>17</v>
@@ -3436,10 +3445,10 @@
         <v>16</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
@@ -3451,7 +3460,7 @@
         <v>20</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>17</v>
@@ -3460,10 +3469,10 @@
         <v>15</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
@@ -3475,7 +3484,7 @@
         <v>20</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>17</v>
@@ -3487,10 +3496,10 @@
         <v>9</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
@@ -3502,7 +3511,7 @@
         <v>20</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>17</v>
@@ -3514,10 +3523,10 @@
         <v>6</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
@@ -3529,7 +3538,7 @@
         <v>20</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>17</v>
@@ -3541,10 +3550,10 @@
         <v>8</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
@@ -3556,7 +3565,7 @@
         <v>20</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>17</v>
@@ -3568,10 +3577,10 @@
         <v>17</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
@@ -3583,7 +3592,7 @@
         <v>20</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>17</v>
@@ -3595,10 +3604,10 @@
         <v>11</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
@@ -3610,7 +3619,7 @@
         <v>20</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>17</v>
@@ -3622,10 +3631,10 @@
         <v>12</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
@@ -3637,7 +3646,7 @@
         <v>20</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>17</v>
@@ -3646,13 +3655,13 @@
         <v>15</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
@@ -3664,19 +3673,19 @@
         <v>20</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
@@ -3688,16 +3697,16 @@
         <v>20</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
@@ -3709,7 +3718,7 @@
         <v>20</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>16</v>
@@ -3718,10 +3727,10 @@
         <v>18</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
@@ -3733,7 +3742,7 @@
         <v>20</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>16</v>
@@ -3742,10 +3751,10 @@
         <v>6</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
@@ -3757,7 +3766,7 @@
         <v>20</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>16</v>
@@ -3766,10 +3775,10 @@
         <v>8</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
@@ -3781,7 +3790,7 @@
         <v>20</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>16</v>
@@ -3790,10 +3799,10 @@
         <v>17</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
@@ -3805,7 +3814,7 @@
         <v>20</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>16</v>
@@ -3814,10 +3823,10 @@
         <v>11</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
@@ -3829,19 +3838,19 @@
         <v>20</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
@@ -3853,16 +3862,16 @@
         <v>20</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
@@ -3874,7 +3883,7 @@
         <v>20</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -3883,10 +3892,10 @@
         <v>8</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
@@ -3898,7 +3907,7 @@
         <v>20</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>11</v>
@@ -3907,10 +3916,10 @@
         <v>13</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
@@ -3922,7 +3931,7 @@
         <v>20</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>11</v>
@@ -3934,10 +3943,10 @@
         <v>9</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="K106" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
@@ -3949,7 +3958,7 @@
         <v>20</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -3961,10 +3970,10 @@
         <v>6</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
@@ -3976,7 +3985,7 @@
         <v>20</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>11</v>
@@ -3988,10 +3997,10 @@
         <v>8</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
@@ -4003,7 +4012,7 @@
         <v>20</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
@@ -4015,10 +4024,10 @@
         <v>14</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
@@ -4030,7 +4039,7 @@
         <v>20</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -4042,10 +4051,10 @@
         <v>15</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
@@ -4057,7 +4066,7 @@
         <v>20</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -4069,10 +4078,10 @@
         <v>17</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
@@ -4084,7 +4093,7 @@
         <v>20</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>11</v>
@@ -4096,10 +4105,10 @@
         <v>16</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
@@ -4111,7 +4120,7 @@
         <v>20</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -4123,10 +4132,10 @@
         <v>11</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
@@ -4138,7 +4147,7 @@
         <v>20</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -4147,13 +4156,13 @@
         <v>13</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
@@ -4165,7 +4174,7 @@
         <v>20</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -4174,10 +4183,10 @@
         <v>17</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
@@ -4189,7 +4198,7 @@
         <v>20</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -4198,10 +4207,10 @@
         <v>12</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
@@ -4213,19 +4222,19 @@
         <v>20</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
@@ -4237,16 +4246,16 @@
         <v>20</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">
@@ -4258,7 +4267,7 @@
         <v>20</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>12</v>
@@ -4267,10 +4276,10 @@
         <v>18</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
@@ -4282,7 +4291,7 @@
         <v>20</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>12</v>
@@ -4294,10 +4303,10 @@
         <v>17</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
@@ -4309,7 +4318,7 @@
         <v>20</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>12</v>
@@ -4321,10 +4330,10 @@
         <v>11</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
@@ -4336,7 +4345,7 @@
         <v>20</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>12</v>
@@ -4348,10 +4357,10 @@
         <v>12</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
@@ -4363,7 +4372,7 @@
         <v>20</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>12</v>
@@ -4372,10 +4381,10 @@
         <v>6</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
@@ -4387,7 +4396,7 @@
         <v>20</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>12</v>
@@ -4399,10 +4408,10 @@
         <v>6</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="K124" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.2">
@@ -4414,7 +4423,7 @@
         <v>20</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>12</v>
@@ -4426,10 +4435,10 @@
         <v>15</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
@@ -4441,7 +4450,7 @@
         <v>20</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>12</v>
@@ -4450,13 +4459,13 @@
         <v>6</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J126" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="K126" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
@@ -4468,16 +4477,16 @@
         <v>20</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.2">
@@ -4489,19 +4498,19 @@
         <v>20</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J128" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.2">
@@ -4513,19 +4522,19 @@
         <v>20</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J129" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.2">
@@ -4537,19 +4546,19 @@
         <v>20</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J130" s="1" t="s">
-        <v>147</v>
+        <v>276</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>